<commit_message>
updated files till today
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/Registration.xlsx
+++ b/src/main/resources/testData/Registration.xlsx
@@ -1,13 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D92B5D-8D68-407A-97BA-EA01EB9DE8B6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="5190" windowWidth="20460" windowHeight="10890"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
+    <sheet name="DuplicateRegis" sheetId="2" r:id="rId2"/>
+    <sheet name="MandatoryFields" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
     <t>runMode</t>
   </si>
@@ -51,12 +54,6 @@
     <t>ConPassword</t>
   </si>
   <si>
-    <t>Foster</t>
-  </si>
-  <si>
-    <t>Guinnesse</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -69,13 +66,49 @@
     <t>UK National</t>
   </si>
   <si>
-    <t>pankaj.missguided145@gmail.com</t>
+    <t>ThankyouText</t>
+  </si>
+  <si>
+    <t>Confirmation has been sent to your email address.</t>
+  </si>
+  <si>
+    <t>ConfirmationText</t>
+  </si>
+  <si>
+    <t>Continue with application</t>
+  </si>
+  <si>
+    <t>ContinueButtonText</t>
+  </si>
+  <si>
+    <t>Thank you for creating a user account.</t>
+  </si>
+  <si>
+    <t>WelcomeText</t>
+  </si>
+  <si>
+    <t>Grant</t>
+  </si>
+  <si>
+    <t>Howard</t>
+  </si>
+  <si>
+    <t>Welcome Howard</t>
+  </si>
+  <si>
+    <t>pankaj.missguided1354@gmail.com</t>
+  </si>
+  <si>
+    <t>ErrorMsg</t>
+  </si>
+  <si>
+    <t>A person with the same details already has a user account. If you know your username and password, select 'Log on' below. If you need assistance, select 'Forgot password?'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -399,25 +432,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E1" sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.88671875" customWidth="1"/>
+    <col min="11" max="12" width="24.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -443,43 +479,193 @@
         <v>9</v>
       </c>
       <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="K2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B13014D-3625-4D9C-8CF7-AB093221ACDE}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{D6A8C6E9-CC1B-438C-9EB7-918BB2C1D392}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56BAC54B-75FA-420A-9E4C-6E2BBE8C2605}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>